<commit_message>
Example Acoustic Pollution and Public Bus
Update specification Public Bus and example Acoustic Pollution
</commit_message>
<xml_diff>
--- a/examples/publicBus/input/InputBusRuta.xlsx
+++ b/examples/publicBus/input/InputBusRuta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/publicBus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/publicBus/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A095823B-5C95-F34E-AE81-251B7EF8686F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3CF1D7-81FB-0243-98AE-5B334396283A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="620" windowWidth="30900" windowHeight="18140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,7 +437,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -467,6 +467,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -485,10 +493,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -511,8 +520,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1290,7 +1301,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,7 +1383,7 @@
       <c r="B7" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="12" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1432,6 +1443,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{B829F4EB-E768-A842-9FC9-226305AE3987}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1442,7 +1456,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1815,7 +1829,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>

</xml_diff>